<commit_message>
Update Bill of Materials
Battery research
</commit_message>
<xml_diff>
--- a/Bill of Materials.xlsx
+++ b/Bill of Materials.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jovanny\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\BAJA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7650" xr2:uid="{DA5A5263-F4D8-4AD9-8F50-968DC5C3F64A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{DA5A5263-F4D8-4AD9-8F50-968DC5C3F64A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="129">
   <si>
     <t>500kg load cell</t>
   </si>
@@ -85,6 +86,15 @@
     <t>http://www.robotshop.com/en/500kg-s-type-load-cell.html</t>
   </si>
   <si>
+    <t>robotshop</t>
+  </si>
+  <si>
+    <t>sparkfun</t>
+  </si>
+  <si>
+    <t>adafruit</t>
+  </si>
+  <si>
     <t>http://www.robotshop.com/en/strain-gauge-load-cell-amplifier-shield-2ch.html</t>
   </si>
   <si>
@@ -142,6 +152,9 @@
     <t>Saving recorded data</t>
   </si>
   <si>
+    <t>http://www.robotshop.com/en/magnet-8-x-3mm-10pk.html</t>
+  </si>
+  <si>
     <t>Magnets(10pk)</t>
   </si>
   <si>
@@ -169,9 +182,6 @@
     <t>None</t>
   </si>
   <si>
-    <t>External 9V</t>
-  </si>
-  <si>
     <t>Computer Fan</t>
   </si>
   <si>
@@ -190,9 +200,15 @@
     <t>PC Hub</t>
   </si>
   <si>
+    <t>arduino</t>
+  </si>
+  <si>
     <t>http://www.orvac.com/Catalog/Push-Button/218975.html</t>
   </si>
   <si>
+    <t>orvac electronics</t>
+  </si>
+  <si>
     <t>Push Button</t>
   </si>
   <si>
@@ -235,64 +251,178 @@
     <t>Terminal Block</t>
   </si>
   <si>
-    <t>Part No.</t>
-  </si>
-  <si>
-    <t>30-10062</t>
-  </si>
-  <si>
-    <t>grm80-30</t>
-  </si>
-  <si>
-    <t>ntebu:25-e100-0</t>
-  </si>
-  <si>
-    <t>Harbor Freight</t>
-  </si>
-  <si>
-    <t>https://www.harborfreight.com/10-piece-rare-earth-magnets-67488.html</t>
-  </si>
-  <si>
-    <t>Arduino Stackable Header Kit</t>
-  </si>
-  <si>
-    <t>RobotShop.com</t>
-  </si>
-  <si>
-    <t>http://www.robotshop.com/en/arduino-mega-stackable-header-kit.html</t>
-  </si>
-  <si>
-    <t>Arduino Shield</t>
-  </si>
-  <si>
-    <t>Arduino Stackable 10-pin header (4pk)</t>
-  </si>
-  <si>
-    <t>http://www.robotshop.com/en/arduino-stackable-header-10-pin-4pk.html</t>
-  </si>
-  <si>
-    <t>http://www.robotshop.com/en/elenco-22-gauge-black-25-ft.html</t>
-  </si>
-  <si>
-    <t>Hook Up Wire (Bk/W/R)</t>
-  </si>
-  <si>
-    <t>Luis Orozco</t>
-  </si>
-  <si>
-    <t>Orvac Electronics</t>
-  </si>
-  <si>
-    <t>Sparkfun.com</t>
-  </si>
-  <si>
-    <t>Adafruit.com</t>
-  </si>
-  <si>
-    <t>Arduino</t>
-  </si>
-  <si>
-    <t>Reimbursable:</t>
+    <t>https://www.amazon.com/eBoot-LM2596-Converter-3-0-40V-1-5-35V/dp/B01GJ0SC2C/ref=sr_1_1_sspa?ie=UTF8&amp;qid=1507863050&amp;sr=8-1-spons&amp;keywords=buck+converter&amp;psc=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Battery Options</t>
+  </si>
+  <si>
+    <t>Sealed Lead Acid</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>1.7lbs</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>6V</t>
+  </si>
+  <si>
+    <t>Battery Clerk</t>
+  </si>
+  <si>
+    <t>Voltage</t>
+  </si>
+  <si>
+    <t>Amp Hours</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>12v</t>
+  </si>
+  <si>
+    <t>Battery Sharks</t>
+  </si>
+  <si>
+    <t>Lithium Ion</t>
+  </si>
+  <si>
+    <t>Pros</t>
+  </si>
+  <si>
+    <t>Cons</t>
+  </si>
+  <si>
+    <t>durability</t>
+  </si>
+  <si>
+    <t>inexpensive</t>
+  </si>
+  <si>
+    <t>rechargable</t>
+  </si>
+  <si>
+    <t>low capacity</t>
+  </si>
+  <si>
+    <t>heavy and large</t>
+  </si>
+  <si>
+    <t>low maintenace</t>
+  </si>
+  <si>
+    <t>rechargeable</t>
+  </si>
+  <si>
+    <t>high maintenance</t>
+  </si>
+  <si>
+    <t>lightweight</t>
+  </si>
+  <si>
+    <t>reconfigurable</t>
+  </si>
+  <si>
+    <t>small</t>
+  </si>
+  <si>
+    <t>expensive</t>
+  </si>
+  <si>
+    <t>adjustable capacity</t>
+  </si>
+  <si>
+    <t>batteryspace.com</t>
+  </si>
+  <si>
+    <t>4.8lbs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width </t>
+  </si>
+  <si>
+    <t>Dimensions</t>
+  </si>
+  <si>
+    <t>18.5mm</t>
+  </si>
+  <si>
+    <t>2.8in</t>
+  </si>
+  <si>
+    <t>5.95in</t>
+  </si>
+  <si>
+    <t>1.9in</t>
+  </si>
+  <si>
+    <t>2.56in</t>
+  </si>
+  <si>
+    <t>4.1in</t>
+  </si>
+  <si>
+    <t>3.7in</t>
+  </si>
+  <si>
+    <t>65.3mm</t>
+  </si>
+  <si>
+    <t>3.6V(10.8V)</t>
+  </si>
+  <si>
+    <t>slow charging (~8hrs)</t>
+  </si>
+  <si>
+    <t>fast charge</t>
+  </si>
+  <si>
+    <t>3.35*</t>
+  </si>
+  <si>
+    <t>*battery management system</t>
+  </si>
+  <si>
+    <t>48.5g(0.3lbs)</t>
+  </si>
+  <si>
+    <t>3.7V(11.1V)</t>
+  </si>
+  <si>
+    <t>2.2(6.6)</t>
+  </si>
+  <si>
+    <t>eBay(10 pack)</t>
+  </si>
+  <si>
+    <t>Minimum runtime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 hours </t>
+  </si>
+  <si>
+    <t>4 hours</t>
+  </si>
+  <si>
+    <t>8 hours</t>
+  </si>
+  <si>
+    <t>5 hours</t>
+  </si>
+  <si>
+    <t>&lt;1lb</t>
   </si>
 </sst>
 </file>
@@ -332,7 +462,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -347,7 +477,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -366,7 +508,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
@@ -379,7 +521,29 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -696,10 +860,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE38B4DA-7DE4-4309-AC06-0721A144F80B}">
-  <dimension ref="B1:L28"/>
+  <dimension ref="B1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,15 +871,15 @@
     <col min="2" max="2" width="20.28515625" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
     <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
     <col min="8" max="8" width="24" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -724,7 +888,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
@@ -735,7 +899,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>13</v>
@@ -744,16 +908,20 @@
         <v>14</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="4">
+        <f>SUM(E3:E22)</f>
+        <v>212.32999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -768,19 +936,19 @@
         <v>50</v>
       </c>
       <c r="F3" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="I3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -795,100 +963,100 @@
         <v>19.95</v>
       </c>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="4">
         <v>0.95</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="3">
         <v>2</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="4">
         <f t="shared" si="0"/>
         <v>1.9</v>
       </c>
-      <c r="F5" t="s">
-        <v>82</v>
-      </c>
-      <c r="G5" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="G5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="13">
         <v>7.5</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="12">
         <v>1</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="13">
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
-      <c r="F6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
+      <c r="F6" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="4">
         <v>14.95</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="3">
         <v>1</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="4">
         <f>C7*D7</f>
         <v>14.95</v>
       </c>
-      <c r="F7" t="s">
-        <v>82</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -903,130 +1071,127 @@
         <v>5.25</v>
       </c>
       <c r="F8" t="s">
-        <v>82</v>
+        <v>17</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H8" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="I8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="4">
         <v>3.5</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="3">
         <v>2</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="4">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="F9" t="s">
-        <v>73</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
+      <c r="F9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="1">
         <v>2.95</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10">
         <v>2</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="1">
         <f t="shared" si="1"/>
         <v>5.9</v>
       </c>
       <c r="F10" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="I10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="8">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="1">
         <v>3.19</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11">
         <v>2</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="1">
         <f t="shared" si="1"/>
         <v>6.38</v>
       </c>
       <c r="F11" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="H11" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I11" t="s">
-        <v>43</v>
-      </c>
-      <c r="J11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" s="8">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="1">
         <v>0.35</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12">
         <v>3</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="1">
         <f t="shared" si="1"/>
         <v>1.0499999999999998</v>
       </c>
       <c r="F12" t="s">
-        <v>82</v>
+        <v>17</v>
       </c>
       <c r="G12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" t="s">
         <v>36</v>
       </c>
-      <c r="H12" t="s">
-        <v>33</v>
-      </c>
       <c r="I12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>4</v>
       </c>
@@ -1038,15 +1203,15 @@
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="I13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1056,290 +1221,193 @@
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="I14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="1"/>
+        <v>4.3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="8">
-        <v>2.99</v>
-      </c>
-      <c r="D15" s="7">
+      <c r="C16" s="10">
+        <v>38.5</v>
+      </c>
+      <c r="D16" s="9">
         <v>1</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E16" s="10">
         <f t="shared" si="1"/>
-        <v>2.99</v>
-      </c>
-      <c r="F15" t="s">
-        <v>70</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0</v>
-      </c>
-      <c r="D16">
+        <v>38.5</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="10">
+        <v>23.39</v>
+      </c>
+      <c r="D17" s="9">
         <v>1</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E17" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F16" t="s">
-        <v>84</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H16" t="s">
-        <v>40</v>
-      </c>
-      <c r="I16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0</v>
-      </c>
-      <c r="D17">
+        <v>23.39</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2.69</v>
+      </c>
+      <c r="D18">
         <v>1</v>
       </c>
-      <c r="E17" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F17" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H17" t="s">
-        <v>46</v>
-      </c>
-      <c r="I17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="8">
-        <v>2.69</v>
-      </c>
-      <c r="D18" s="7">
-        <v>1</v>
-      </c>
-      <c r="E18" s="8">
+      <c r="E18" s="1">
         <f t="shared" si="1"/>
         <v>2.69</v>
       </c>
       <c r="F18" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="H18" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="I18" t="s">
-        <v>43</v>
-      </c>
-      <c r="J18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="1">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H19" t="s">
+        <v>65</v>
+      </c>
+      <c r="I19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="1">
+        <v>11.59</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="1"/>
+        <v>11.59</v>
+      </c>
+      <c r="F20" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="8">
-        <v>20</v>
-      </c>
-      <c r="D19" s="7">
-        <v>1</v>
-      </c>
-      <c r="E19" s="8">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="F19" t="s">
-        <v>80</v>
-      </c>
-      <c r="H19" t="s">
-        <v>60</v>
-      </c>
-      <c r="I19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="8">
-        <v>11</v>
-      </c>
-      <c r="D20" s="7">
-        <v>1</v>
-      </c>
-      <c r="E20" s="8">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="F20" t="s">
-        <v>62</v>
-      </c>
-      <c r="H20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E21" s="1">
         <f>C21*D21</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" s="8">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="1">
         <v>0.99</v>
       </c>
-      <c r="D22" s="7">
-        <v>5</v>
-      </c>
-      <c r="E22" s="8">
-        <f t="shared" ref="E22:E25" si="2">C22*D22</f>
-        <v>4.95</v>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" ref="E22" si="2">C22*D22</f>
+        <v>1.98</v>
       </c>
       <c r="F22" t="s">
-        <v>81</v>
-      </c>
-      <c r="J22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" t="s">
         <v>72</v>
-      </c>
-      <c r="C23" s="8">
-        <v>1.99</v>
-      </c>
-      <c r="D23" s="7">
-        <v>2</v>
-      </c>
-      <c r="E23" s="8">
-        <f t="shared" si="2"/>
-        <v>3.98</v>
-      </c>
-      <c r="F23" t="s">
-        <v>73</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H23" t="s">
-        <v>75</v>
-      </c>
-      <c r="I23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C24" s="8">
-        <v>1.31</v>
-      </c>
-      <c r="D24" s="7">
-        <v>1</v>
-      </c>
-      <c r="E24" s="8">
-        <f t="shared" si="2"/>
-        <v>1.31</v>
-      </c>
-      <c r="F24" t="s">
-        <v>73</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H24" t="s">
-        <v>75</v>
-      </c>
-      <c r="I24" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C25" s="8">
-        <v>2.25</v>
-      </c>
-      <c r="D25" s="7">
-        <v>3</v>
-      </c>
-      <c r="E25" s="8">
-        <f t="shared" si="2"/>
-        <v>6.75</v>
-      </c>
-      <c r="F25" t="s">
-        <v>73</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="H25" t="s">
-        <v>75</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L25" s="4">
-        <f>SUM(E3:E25)</f>
-        <v>173.54999999999998</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="E28" s="1">
-        <f>SUM(E5,E6,E7,E9,E10,E11,E12,E15,E18,E19,E20,E22:E25)</f>
-        <v>98.350000000000009</v>
       </c>
     </row>
   </sheetData>
@@ -1356,15 +1424,338 @@
     <hyperlink ref="G9" r:id="rId7" xr:uid="{25E7E0B1-8F00-4413-B442-55693A7BE4F7}"/>
     <hyperlink ref="G10" r:id="rId8" xr:uid="{DC169C43-5AB6-4670-B456-990B68233B9E}"/>
     <hyperlink ref="G11" r:id="rId9" xr:uid="{72D1C858-F407-4608-94B1-A68BF56AEC2C}"/>
-    <hyperlink ref="G12" r:id="rId10" xr:uid="{A693F035-CA40-45EB-B471-E05D6BCC198C}"/>
-    <hyperlink ref="G16" r:id="rId11" xr:uid="{384B4B0F-91A9-493E-BAE4-CF4A7F1007B8}"/>
-    <hyperlink ref="G17" r:id="rId12" xr:uid="{D964BCCA-8F50-4EB0-8B5B-284F3524A5C4}"/>
-    <hyperlink ref="G18" r:id="rId13" xr:uid="{4FE019D7-ADCF-4598-BA12-0F28849D1C6A}"/>
-    <hyperlink ref="G23" r:id="rId14" xr:uid="{D525C2D6-5274-4537-93DE-61024A9E6610}"/>
-    <hyperlink ref="G24" r:id="rId15" xr:uid="{B9AEAAA7-F866-45FE-ACA1-5A60D07A64D8}"/>
-    <hyperlink ref="G25" r:id="rId16" xr:uid="{369ADC7C-E7DC-40A1-ACD1-04782E84449B}"/>
+    <hyperlink ref="G15" r:id="rId10" xr:uid="{09BEBB27-8858-4F6F-B29B-E1496C5E000F}"/>
+    <hyperlink ref="G12" r:id="rId11" xr:uid="{A693F035-CA40-45EB-B471-E05D6BCC198C}"/>
+    <hyperlink ref="G16" r:id="rId12" xr:uid="{384B4B0F-91A9-493E-BAE4-CF4A7F1007B8}"/>
+    <hyperlink ref="G17" r:id="rId13" xr:uid="{D964BCCA-8F50-4EB0-8B5B-284F3524A5C4}"/>
+    <hyperlink ref="G18" r:id="rId14" xr:uid="{4FE019D7-ADCF-4598-BA12-0F28849D1C6A}"/>
+    <hyperlink ref="G20" r:id="rId15" xr:uid="{8DEE3598-4281-4B53-863F-44E9F1109489}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D8CDD5-30AA-4B63-A51E-E099D7AD43BE}">
+  <dimension ref="B2:M22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" customWidth="1"/>
+    <col min="15" max="15" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E3" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="15">
+        <v>4.5</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="I5" s="15">
+        <v>5.89</v>
+      </c>
+      <c r="J5" s="15">
+        <v>4</v>
+      </c>
+      <c r="K5" s="15">
+        <f>I5*J5</f>
+        <v>23.56</v>
+      </c>
+      <c r="L5" t="s">
+        <v>80</v>
+      </c>
+      <c r="M5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="15">
+        <v>7</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="I6" s="15">
+        <v>9.9700000000000006</v>
+      </c>
+      <c r="J6" s="15">
+        <v>2</v>
+      </c>
+      <c r="K6" s="15">
+        <f t="shared" ref="K6:K7" si="0">I6*J6</f>
+        <v>19.940000000000001</v>
+      </c>
+      <c r="L6" t="s">
+        <v>85</v>
+      </c>
+      <c r="M6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="I7" s="15">
+        <v>13.95</v>
+      </c>
+      <c r="J7" s="15">
+        <v>3</v>
+      </c>
+      <c r="K7" s="15">
+        <f>I7*J7</f>
+        <v>41.849999999999994</v>
+      </c>
+      <c r="L7" t="s">
+        <v>102</v>
+      </c>
+      <c r="M7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="I8" s="19">
+        <v>26.98</v>
+      </c>
+      <c r="J8" s="19">
+        <v>1</v>
+      </c>
+      <c r="K8" s="19">
+        <f>I8*J8</f>
+        <v>26.98</v>
+      </c>
+      <c r="L8" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="M8" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="J9" s="15"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C10" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E3:G3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>